<commit_message>
Experiment 2 and mstatistical interpretations
</commit_message>
<xml_diff>
--- a/Exp1_AnalysisData.xlsx
+++ b/Exp1_AnalysisData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shevyapanda/Desktop/personalprojects/PALS_Projects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{832B886B-42F3-544A-954E-14039CE2FDED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BEF2C62-17A1-E444-B7DF-77880302BC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="1460" windowWidth="27640" windowHeight="15680" xr2:uid="{7D04B8E7-D956-7B45-BC43-D2728EE71451}"/>
+    <workbookView xWindow="1160" yWindow="800" windowWidth="27640" windowHeight="15680" xr2:uid="{7D04B8E7-D956-7B45-BC43-D2728EE71451}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -561,7 +561,7 @@
   <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>